<commit_message>
Add nakshatra and nakshatra lord to asc, timezone in wordings updated (possible convert to gmt)
</commit_message>
<xml_diff>
--- a/nameoftheperson_chartgen.xlsx
+++ b/nameoftheperson_chartgen.xlsx
@@ -437,7 +437,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Thanushurgr8</t>
+          <t>Thanush_Test</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>19/08/1999</t>
+          <t>10/05/1999</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>03:02:09</t>
+          <t>03:04:00</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>tobefilled GMT+5.5</t>
+          <t>Asia/Kolkata</t>
         </is>
       </c>
     </row>
@@ -607,7 +607,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Retro</t>
+          <t>Retro(R)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -639,26 +639,26 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Gemini</t>
+          <t>Pisces</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mercury</t>
+          <t>Jupiter</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>Purva Bhadrapada</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>Jupiter</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>15.87253558834242</v>
+        <v>1.263900747942614</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -692,26 +692,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Leo</t>
+          <t>Aries</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Magha</t>
+          <t>Bharani</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Ketu</t>
+          <t>Venus</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>121.6464808771245</v>
+        <v>24.96816340468312</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -729,7 +729,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -745,26 +745,26 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Libra</t>
+          <t>Aquarius</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Venus</t>
+          <t>Saturn</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Vishakha</t>
+          <t>Shatabhisha</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Jupiter</t>
+          <t>Rahu</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>209.7082810541858</v>
+        <v>309.075052640371</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -798,26 +798,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cancer</t>
+          <t>Aries</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Moon</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Pushya</t>
+          <t>Ashwini</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Saturn</t>
+          <t>Ketu</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>103.7480180076092</v>
+        <v>7.96109256468479</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -851,35 +851,35 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Leo</t>
+          <t>Gemini</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Mercury</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Magha</t>
+          <t>Ardra</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Ketu</t>
+          <t>Rahu</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>124.1791905532752</v>
+        <v>67.50609350739118</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Retro</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Combust</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -888,7 +888,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -914,20 +914,20 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Vishakha</t>
+          <t>Chitra</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Jupiter</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>207.1803783902383</v>
+        <v>184.8265144931989</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Retro</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -957,26 +957,26 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Aries</t>
+          <t>Pisces</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Jupiter</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Ashwini</t>
+          <t>Revati</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ketu</t>
+          <t>Mercury</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>11.07444566281574</v>
+        <v>356.3771724279898</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -1029,7 +1029,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>23.22205786413803</v>
+        <v>14.49292394624836</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Combust</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -1082,11 +1082,11 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>290.5271832388229</v>
+        <v>292.8890339183791</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Retro</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1100,7 +1100,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -1126,16 +1126,16 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Uttara Ashadha</t>
+          <t>Shravana</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Moon</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>278.5111603261211</v>
+        <v>280.5216800641753</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -1188,7 +1188,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>223.8890396348532</v>
+        <v>225.8449774019211</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1206,7 +1206,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1241,7 +1241,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>108.3732820467913</v>
+        <v>113.7254071935777</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1285,16 +1285,16 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Shravana</t>
+          <t>Dhanishta</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Moon</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>289.0222711812717</v>
+        <v>293.560692356362</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>

</xml_diff>